<commit_message>
Analisis de unicidad completado
</commit_message>
<xml_diff>
--- a/proyecto/SimbolTable.xlsx
+++ b/proyecto/SimbolTable.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chuzd\Compiladores\proyecto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40D6A072-78A7-4F91-B80F-B8FF0516658C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9485F22A-60E4-48B6-BD7F-61CD184FE620}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="87">
   <si>
     <t>class Program {</t>
   </si>
@@ -99,15 +99,6 @@
   </si>
   <si>
     <t xml:space="preserve">    void daniel() {</t>
-  </si>
-  <si>
-    <t>False</t>
-  </si>
-  <si>
-    <t>Variable</t>
-  </si>
-  <si>
-    <t>True</t>
   </si>
   <si>
     <t>Var Declaration</t>
@@ -349,9 +340,6 @@
     <t>Agregar Char Literal ""</t>
   </si>
   <si>
-    <t xml:space="preserve">Modificar el Sintax Cup, añadir location a ID </t>
-  </si>
-  <si>
     <t>Crear la tabla de simbolos</t>
   </si>
   <si>
@@ -371,13 +359,141 @@
   </si>
   <si>
     <t>RDS rstudio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Size </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Method </t>
+  </si>
+  <si>
+    <t xml:space="preserve">True </t>
+  </si>
+  <si>
+    <t xml:space="preserve">False </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tabla de Métodos </t>
+  </si>
+  <si>
+    <t>Input Vars</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Modificar el Sintax Cup, añadir identifier y location a ID </t>
+  </si>
+  <si>
+    <t xml:space="preserve">CharLiteral </t>
+  </si>
+  <si>
+    <t>Variables input</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DecimalLiteral </t>
+  </si>
+  <si>
+    <t>HexLiteral</t>
+  </si>
+  <si>
+    <r>
+      <t>private</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF569CD6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>String</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> identifier; </t>
+    </r>
+  </si>
+  <si>
+    <t>CheckList</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nombre </t>
+  </si>
+  <si>
+    <t xml:space="preserve">valor </t>
+  </si>
+  <si>
+    <t xml:space="preserve">numNodo </t>
+  </si>
+  <si>
+    <t>identifier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">location </t>
+  </si>
+  <si>
+    <t xml:space="preserve">hijos </t>
+  </si>
+  <si>
+    <t xml:space="preserve">NoNull </t>
+  </si>
+  <si>
+    <t xml:space="preserve">NULL </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Variables input </t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Terminamos con un {  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">    void funcion(int a, int b, boolen f) {</t>
+  </si>
+  <si>
+    <t>nombres</t>
+  </si>
+  <si>
+    <t>scope</t>
+  </si>
+  <si>
+    <t>ArrayList</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>z</t>
+  </si>
+  <si>
+    <t>j</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -433,8 +549,31 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00B0F0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -447,8 +586,26 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC00000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -471,11 +628,102 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -502,6 +750,35 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -532,7 +809,7 @@
       <xdr:col>19</xdr:col>
       <xdr:colOff>458688</xdr:colOff>
       <xdr:row>41</xdr:row>
-      <xdr:rowOff>3899</xdr:rowOff>
+      <xdr:rowOff>679</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -769,16 +1046,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>35</xdr:col>
-      <xdr:colOff>132037</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>171237</xdr:rowOff>
+      <xdr:col>39</xdr:col>
+      <xdr:colOff>104823</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>7952</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>36</xdr:col>
-      <xdr:colOff>103813</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>79515</xdr:rowOff>
+      <xdr:col>40</xdr:col>
+      <xdr:colOff>76598</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>97658</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -793,8 +1070,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="22008364" y="711564"/>
-          <a:ext cx="581376" cy="268496"/>
+          <a:off x="24697466" y="370809"/>
+          <a:ext cx="579561" cy="271135"/>
         </a:xfrm>
         <a:prstGeom prst="leftArrow">
           <a:avLst/>
@@ -830,15 +1107,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>23</xdr:col>
-      <xdr:colOff>303734</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>168875</xdr:rowOff>
+      <xdr:colOff>487281</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>121597</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>24</xdr:col>
-      <xdr:colOff>272689</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>77154</xdr:rowOff>
+      <xdr:colOff>456236</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>29876</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -853,8 +1130,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="14324534" y="531340"/>
-          <a:ext cx="578555" cy="270744"/>
+          <a:off x="14495288" y="855787"/>
+          <a:ext cx="577999" cy="275374"/>
         </a:xfrm>
         <a:prstGeom prst="leftArrow">
           <a:avLst/>
@@ -889,16 +1166,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>296644</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>150444</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>548026</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>32608</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>600832</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>127585</xdr:rowOff>
+      <xdr:colOff>239471</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>9749</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -913,8 +1190,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3943970" y="1229231"/>
-          <a:ext cx="304188" cy="336736"/>
+          <a:off x="3611737" y="1297371"/>
+          <a:ext cx="304188" cy="338502"/>
         </a:xfrm>
         <a:prstGeom prst="downArrow">
           <a:avLst/>
@@ -1197,8 +1474,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="13669896" y="64827"/>
-          <a:ext cx="304188" cy="339605"/>
+          <a:off x="13669896" y="1697684"/>
+          <a:ext cx="304188" cy="339997"/>
         </a:xfrm>
         <a:prstGeom prst="downArrow">
           <a:avLst/>
@@ -1723,6 +2000,127 @@
             <a:rPr lang="es-GT" sz="1100" baseline="0"/>
             <a:t>Variable  </a:t>
           </a:r>
+          <a:endParaRPr lang="es-GT" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>393095</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>36</xdr:col>
+      <xdr:colOff>580571</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>102809</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="17" name="Conector recto de flecha 16">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D6F7A13B-E4D0-5FE2-283B-030F0ECC5D3F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="22388285" y="6839857"/>
+          <a:ext cx="1058334" cy="169333"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>33</xdr:col>
+      <xdr:colOff>93689</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>56213</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>33</xdr:col>
+      <xdr:colOff>397877</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>33353</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="24" name="Flecha: hacia abajo 23">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{62BE048A-87D5-4307-8015-D2E45958D76F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="10800000">
+          <a:off x="20898787" y="10586803"/>
+          <a:ext cx="304188" cy="339402"/>
+        </a:xfrm>
+        <a:prstGeom prst="downArrow">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent2"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="0070C0"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
           <a:endParaRPr lang="es-GT" sz="1100"/>
         </a:p>
       </xdr:txBody>
@@ -1995,10 +2393,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:AQ52"/>
+  <dimension ref="B2:AR71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="V36" zoomScale="125" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AB52" sqref="AB52"/>
+    <sheetView tabSelected="1" topLeftCell="U44" zoomScale="122" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AG62" sqref="AG62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2007,9 +2405,11 @@
     <col min="27" max="27" width="11.21875" customWidth="1"/>
     <col min="28" max="28" width="11" customWidth="1"/>
     <col min="30" max="30" width="10.5546875" customWidth="1"/>
+    <col min="36" max="36" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="9.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:44" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
         <v>6</v>
       </c>
@@ -2023,7 +2423,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:44" x14ac:dyDescent="0.3">
       <c r="V3" t="s">
         <v>0</v>
       </c>
@@ -2045,28 +2445,31 @@
       <c r="AH3" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="AI3" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="AM3" s="2">
+      <c r="AI3" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="AJ3" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="AN3" s="2">
         <v>2</v>
       </c>
-      <c r="AN3" s="2" t="s">
+      <c r="AO3" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="AO3" s="2" t="s">
+      <c r="AP3" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="AP3" s="2">
+      <c r="AQ3" s="2">
         <v>2</v>
       </c>
-      <c r="AQ3" s="2">
+      <c r="AR3" s="2">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:44" x14ac:dyDescent="0.3">
       <c r="V4" t="s">
-        <v>1</v>
+        <v>78</v>
       </c>
       <c r="Z4" s="4">
         <v>2</v>
@@ -2086,26 +2489,30 @@
       <c r="AH4" s="4">
         <v>2</v>
       </c>
-      <c r="AI4" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="AM4" s="2">
+      <c r="AI4" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="AJ4" s="4">
+        <v>0</v>
+      </c>
+      <c r="AK4" s="3"/>
+      <c r="AN4" s="2">
         <v>3</v>
       </c>
-      <c r="AN4" s="2" t="s">
+      <c r="AO4" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="AO4" s="2" t="s">
+      <c r="AP4" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="AP4" s="2">
+      <c r="AQ4" s="2">
         <v>2</v>
       </c>
-      <c r="AQ4" s="2">
+      <c r="AR4" s="2">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:44" x14ac:dyDescent="0.3">
       <c r="V5" t="s">
         <v>2</v>
       </c>
@@ -2125,75 +2532,148 @@
       <c r="AH5" s="4">
         <v>3</v>
       </c>
-      <c r="AI5" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="AM5" s="2">
+      <c r="AI5" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="AJ5" s="4">
+        <v>0</v>
+      </c>
+      <c r="AK5" s="3"/>
+      <c r="AN5" s="2">
         <v>5</v>
       </c>
-      <c r="AN5" s="2" t="s">
+      <c r="AO5" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="AO5" s="2" t="s">
+      <c r="AP5" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="AP5" s="2">
+      <c r="AQ5" s="2">
         <v>3</v>
       </c>
-      <c r="AQ5" s="2">
+      <c r="AR5" s="2">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:44" x14ac:dyDescent="0.3">
       <c r="V6" t="s">
         <v>3</v>
       </c>
       <c r="Z6" s="4"/>
     </row>
-    <row r="7" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:44" x14ac:dyDescent="0.3">
       <c r="V7" t="s">
         <v>4</v>
       </c>
       <c r="Z7" s="4"/>
     </row>
-    <row r="8" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:44" x14ac:dyDescent="0.3">
       <c r="V8" t="s">
         <v>5</v>
       </c>
       <c r="Z8" s="4"/>
-    </row>
-    <row r="9" spans="2:43" x14ac:dyDescent="0.3">
+      <c r="AD8" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="9" spans="2:44" x14ac:dyDescent="0.3">
       <c r="Z9" s="4"/>
-    </row>
-    <row r="10" spans="2:43" x14ac:dyDescent="0.3">
+      <c r="AD9" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="AE9" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="AF9" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="AG9" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="AH9" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="AI9" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="AJ9" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="AK9" s="16" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="10" spans="2:44" x14ac:dyDescent="0.3">
       <c r="Z10" s="4"/>
-    </row>
-    <row r="11" spans="2:43" x14ac:dyDescent="0.3">
+      <c r="AD10" s="4">
+        <v>1</v>
+      </c>
+      <c r="AE10" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="AF10" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="AG10" s="4">
+        <v>1</v>
+      </c>
+      <c r="AH10" s="4">
+        <v>2</v>
+      </c>
+      <c r="AI10" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="AJ10" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="2:44" x14ac:dyDescent="0.3">
       <c r="V11" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="12" spans="2:43" x14ac:dyDescent="0.3">
+      <c r="AD11" s="4">
+        <v>2</v>
+      </c>
+      <c r="AE11" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="AF11" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="AG11" s="4">
+        <v>2</v>
+      </c>
+      <c r="AH11" s="4">
+        <v>3</v>
+      </c>
+      <c r="AI11" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="AJ11" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="2:44" x14ac:dyDescent="0.3">
       <c r="V12" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:44" x14ac:dyDescent="0.3">
       <c r="V13" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:44" x14ac:dyDescent="0.3">
       <c r="V14" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:44" x14ac:dyDescent="0.3">
       <c r="V15" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:44" x14ac:dyDescent="0.3">
       <c r="V16" t="s">
         <v>4</v>
       </c>
@@ -2201,7 +2681,7 @@
       <c r="AA16" s="3"/>
       <c r="AB16" s="3"/>
     </row>
-    <row r="17" spans="22:40" x14ac:dyDescent="0.3">
+    <row r="17" spans="22:41" x14ac:dyDescent="0.3">
       <c r="V17" t="s">
         <v>20</v>
       </c>
@@ -2209,19 +2689,19 @@
       <c r="AA17" s="5"/>
       <c r="AB17" s="3"/>
     </row>
-    <row r="18" spans="22:40" x14ac:dyDescent="0.3">
+    <row r="18" spans="22:41" x14ac:dyDescent="0.3">
       <c r="V18" t="s">
         <v>2</v>
       </c>
       <c r="Z18" s="8" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="AA18" s="5"/>
-      <c r="AM18" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="19" spans="22:40" x14ac:dyDescent="0.3">
+      <c r="AN18" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="19" spans="22:41" x14ac:dyDescent="0.3">
       <c r="V19" t="s">
         <v>3</v>
       </c>
@@ -2229,25 +2709,25 @@
         <v>1</v>
       </c>
       <c r="AA19" s="7" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="AB19" s="3"/>
       <c r="AE19" s="9" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="AF19" s="10"/>
       <c r="AG19" s="10"/>
       <c r="AI19" t="s">
-        <v>41</v>
-      </c>
-      <c r="AM19">
+        <v>38</v>
+      </c>
+      <c r="AN19">
         <v>1</v>
       </c>
-      <c r="AN19" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="20" spans="22:40" x14ac:dyDescent="0.3">
+      <c r="AO19" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="20" spans="22:41" x14ac:dyDescent="0.3">
       <c r="V20" t="s">
         <v>4</v>
       </c>
@@ -2255,20 +2735,20 @@
         <v>2</v>
       </c>
       <c r="AA20" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="AB20" s="3"/>
       <c r="AI20" t="s">
-        <v>42</v>
-      </c>
-      <c r="AM20">
+        <v>39</v>
+      </c>
+      <c r="AN20">
         <v>2</v>
       </c>
-      <c r="AN20" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="21" spans="22:40" x14ac:dyDescent="0.3">
+      <c r="AO20" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="21" spans="22:41" x14ac:dyDescent="0.3">
       <c r="V21" t="s">
         <v>5</v>
       </c>
@@ -2276,183 +2756,469 @@
         <v>3</v>
       </c>
       <c r="AA21" s="7" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="AB21" s="3"/>
       <c r="AE21" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="AM21">
+        <v>27</v>
+      </c>
+      <c r="AN21">
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="22:40" x14ac:dyDescent="0.3">
+    <row r="22" spans="22:41" x14ac:dyDescent="0.3">
       <c r="Z22" s="6">
         <v>4</v>
       </c>
+      <c r="AA22" s="7" t="s">
+        <v>77</v>
+      </c>
       <c r="AB22" s="3"/>
-    </row>
-    <row r="24" spans="22:40" x14ac:dyDescent="0.3">
+      <c r="AE22" s="9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="24" spans="22:41" x14ac:dyDescent="0.3">
       <c r="Z24" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="25" spans="22:40" x14ac:dyDescent="0.3">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="25" spans="22:41" x14ac:dyDescent="0.3">
       <c r="Z25">
         <v>1</v>
       </c>
       <c r="AA25" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="AE25" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="26" spans="22:40" x14ac:dyDescent="0.3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="26" spans="22:41" x14ac:dyDescent="0.3">
       <c r="Z26">
         <v>2</v>
       </c>
       <c r="AA26" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="AE26" s="9" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="27" spans="22:40" x14ac:dyDescent="0.3">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="27" spans="22:41" x14ac:dyDescent="0.3">
       <c r="Z27">
         <v>3</v>
       </c>
     </row>
-    <row r="30" spans="22:40" x14ac:dyDescent="0.3">
+    <row r="30" spans="22:41" x14ac:dyDescent="0.3">
       <c r="Z30" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="31" spans="22:40" x14ac:dyDescent="0.3">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="31" spans="22:41" x14ac:dyDescent="0.3">
       <c r="AA31" s="11" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="32" spans="22:40" x14ac:dyDescent="0.3">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="32" spans="22:41" x14ac:dyDescent="0.3">
       <c r="AA32" s="12" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="33" spans="26:30" x14ac:dyDescent="0.3">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="33" spans="26:44" x14ac:dyDescent="0.3">
       <c r="AA33" s="12" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="AD33" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="34" spans="26:30" x14ac:dyDescent="0.3">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="34" spans="26:44" x14ac:dyDescent="0.3">
       <c r="AA34" s="12" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="35" spans="26:44" x14ac:dyDescent="0.3">
+      <c r="AA35" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="AD35" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="36" spans="26:44" x14ac:dyDescent="0.3">
+      <c r="AA36" s="13" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="35" spans="26:30" x14ac:dyDescent="0.3">
-      <c r="AA35" s="13" t="s">
-        <v>43</v>
-      </c>
-      <c r="AB35" s="14"/>
-      <c r="AD35" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="36" spans="26:30" x14ac:dyDescent="0.3">
       <c r="AB36" s="14"/>
-    </row>
-    <row r="38" spans="26:30" x14ac:dyDescent="0.3">
+      <c r="AD36" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="38" spans="26:44" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="Z38" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="39" spans="26:30" x14ac:dyDescent="0.3">
+        <v>42</v>
+      </c>
+      <c r="AF38" t="s">
+        <v>66</v>
+      </c>
+      <c r="AI38" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="39" spans="26:44" x14ac:dyDescent="0.3">
       <c r="Z39">
         <v>1</v>
       </c>
       <c r="AA39" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="40" spans="26:30" x14ac:dyDescent="0.3">
+        <v>45</v>
+      </c>
+      <c r="AF39" s="20"/>
+      <c r="AI39" t="s">
+        <v>61</v>
+      </c>
+      <c r="AL39" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="AM39" s="22"/>
+      <c r="AN39" s="29" t="s">
+        <v>75</v>
+      </c>
+      <c r="AP39" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="AQ39" s="22"/>
+      <c r="AR39" s="29" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="40" spans="26:44" x14ac:dyDescent="0.3">
       <c r="Z40">
         <v>2</v>
       </c>
       <c r="AA40" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="41" spans="26:30" x14ac:dyDescent="0.3">
+        <v>46</v>
+      </c>
+      <c r="AF40" s="20"/>
+      <c r="AI40" t="s">
+        <v>63</v>
+      </c>
+      <c r="AL40" s="23"/>
+      <c r="AM40" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="AN40" s="24" t="s">
+        <v>73</v>
+      </c>
+      <c r="AP40" s="23"/>
+      <c r="AQ40" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="AR40" s="24" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="41" spans="26:44" x14ac:dyDescent="0.3">
       <c r="Z41">
         <v>3</v>
       </c>
       <c r="AA41" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="42" spans="26:30" x14ac:dyDescent="0.3">
+        <v>43</v>
+      </c>
+      <c r="AI41" t="s">
+        <v>64</v>
+      </c>
+      <c r="AL41" s="23"/>
+      <c r="AM41" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AN41" s="24" t="s">
+        <v>73</v>
+      </c>
+      <c r="AP41" s="23"/>
+      <c r="AQ41" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AR41" s="24" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="42" spans="26:44" x14ac:dyDescent="0.3">
       <c r="Z42">
         <v>4</v>
       </c>
       <c r="AA42" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="43" spans="26:30" x14ac:dyDescent="0.3">
+        <v>44</v>
+      </c>
+      <c r="AI42" t="s">
+        <v>56</v>
+      </c>
+      <c r="AL42" s="23"/>
+      <c r="AM42" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="AN42" s="24" t="s">
+        <v>73</v>
+      </c>
+      <c r="AP42" s="23"/>
+      <c r="AQ42" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="AR42" s="24" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="43" spans="26:44" x14ac:dyDescent="0.3">
       <c r="Z43">
         <v>5</v>
       </c>
-    </row>
-    <row r="44" spans="26:30" x14ac:dyDescent="0.3">
+      <c r="AI43" t="s">
+        <v>57</v>
+      </c>
+      <c r="AL43" s="23"/>
+      <c r="AM43" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="AN43" s="27" t="s">
+        <v>74</v>
+      </c>
+      <c r="AP43" s="23"/>
+      <c r="AQ43" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="AR43" s="30" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="44" spans="26:44" x14ac:dyDescent="0.3">
       <c r="Z44">
         <v>6</v>
       </c>
       <c r="AA44" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="45" spans="26:30" x14ac:dyDescent="0.3">
+        <v>48</v>
+      </c>
+      <c r="AF44" s="19"/>
+      <c r="AL44" s="23"/>
+      <c r="AM44" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="AN44" s="24" t="s">
+        <v>73</v>
+      </c>
+      <c r="AP44" s="23"/>
+      <c r="AQ44" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="AR44" s="24" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="45" spans="26:44" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="Z45">
         <v>7</v>
       </c>
       <c r="AA45" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="46" spans="26:30" x14ac:dyDescent="0.3">
+        <v>60</v>
+      </c>
+      <c r="AF45" s="20"/>
+      <c r="AL45" s="25"/>
+      <c r="AM45" s="26" t="s">
+        <v>72</v>
+      </c>
+      <c r="AN45" s="28" t="s">
+        <v>74</v>
+      </c>
+      <c r="AP45" s="25"/>
+      <c r="AQ45" s="26" t="s">
+        <v>72</v>
+      </c>
+      <c r="AR45" s="28" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="46" spans="26:44" x14ac:dyDescent="0.3">
       <c r="Z46">
         <v>8</v>
       </c>
       <c r="AA46" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="47" spans="26:44" x14ac:dyDescent="0.3">
+      <c r="AB47" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="47" spans="26:30" x14ac:dyDescent="0.3">
-      <c r="AB47" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="48" spans="26:30" x14ac:dyDescent="0.3">
+    <row r="48" spans="26:44" x14ac:dyDescent="0.3">
       <c r="Z48">
         <v>9</v>
       </c>
       <c r="AA48" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="51" spans="28:28" x14ac:dyDescent="0.3">
+        <v>52</v>
+      </c>
+      <c r="AF48" s="20"/>
+    </row>
+    <row r="51" spans="25:34" x14ac:dyDescent="0.3">
       <c r="AB51" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="52" spans="28:28" x14ac:dyDescent="0.3">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="52" spans="25:34" x14ac:dyDescent="0.3">
       <c r="AB52" s="15"/>
+    </row>
+    <row r="56" spans="25:34" x14ac:dyDescent="0.3">
+      <c r="Y56" t="s">
+        <v>81</v>
+      </c>
+      <c r="Z56" t="s">
+        <v>79</v>
+      </c>
+      <c r="AA56" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="AB56" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="AC56" s="31" t="s">
+        <v>82</v>
+      </c>
+      <c r="AD56" s="33" t="s">
+        <v>83</v>
+      </c>
+      <c r="AE56" s="33" t="s">
+        <v>84</v>
+      </c>
+      <c r="AF56" s="33" t="s">
+        <v>85</v>
+      </c>
+      <c r="AG56" s="33" t="s">
+        <v>86</v>
+      </c>
+      <c r="AH56" s="34" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="57" spans="25:34" x14ac:dyDescent="0.3">
+      <c r="AA57" s="32"/>
+      <c r="AB57" s="32"/>
+      <c r="AC57" s="32"/>
+      <c r="AD57" s="32"/>
+      <c r="AE57" s="32"/>
+      <c r="AF57" s="32"/>
+      <c r="AG57" s="32"/>
+    </row>
+    <row r="58" spans="25:34" x14ac:dyDescent="0.3">
+      <c r="Y58" t="s">
+        <v>81</v>
+      </c>
+      <c r="Z58" t="s">
+        <v>80</v>
+      </c>
+      <c r="AA58" s="31">
+        <v>1</v>
+      </c>
+      <c r="AB58" s="31">
+        <v>1</v>
+      </c>
+      <c r="AC58" s="31">
+        <v>1</v>
+      </c>
+      <c r="AD58" s="33">
+        <v>2</v>
+      </c>
+      <c r="AE58" s="33">
+        <v>2</v>
+      </c>
+      <c r="AF58" s="33">
+        <v>2</v>
+      </c>
+      <c r="AG58" s="33">
+        <v>2</v>
+      </c>
+      <c r="AH58" s="34">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="61" spans="25:34" x14ac:dyDescent="0.3">
+      <c r="AA61" s="4"/>
+      <c r="AB61" s="4"/>
+      <c r="AC61" s="4"/>
+      <c r="AD61" s="4"/>
+      <c r="AE61" s="4"/>
+    </row>
+    <row r="62" spans="25:34" x14ac:dyDescent="0.3">
+      <c r="AA62" s="4"/>
+      <c r="AB62" s="4"/>
+      <c r="AC62" s="4"/>
+      <c r="AD62" s="4"/>
+      <c r="AE62" s="4"/>
+    </row>
+    <row r="63" spans="25:34" x14ac:dyDescent="0.3">
+      <c r="AA63" s="4"/>
+      <c r="AB63" s="4"/>
+      <c r="AC63" s="4"/>
+      <c r="AD63" s="4"/>
+      <c r="AE63" s="4"/>
+    </row>
+    <row r="64" spans="25:34" x14ac:dyDescent="0.3">
+      <c r="AA64" s="4"/>
+      <c r="AB64" s="4"/>
+      <c r="AC64" s="4"/>
+      <c r="AD64" s="4"/>
+      <c r="AE64" s="4"/>
+    </row>
+    <row r="65" spans="27:31" x14ac:dyDescent="0.3">
+      <c r="AA65" s="4"/>
+      <c r="AB65" s="4"/>
+      <c r="AC65" s="4"/>
+      <c r="AD65" s="4"/>
+      <c r="AE65" s="4"/>
+    </row>
+    <row r="66" spans="27:31" x14ac:dyDescent="0.3">
+      <c r="AA66" s="4"/>
+      <c r="AB66" s="4"/>
+      <c r="AC66" s="4"/>
+      <c r="AD66" s="4"/>
+      <c r="AE66" s="4"/>
+    </row>
+    <row r="67" spans="27:31" x14ac:dyDescent="0.3">
+      <c r="AA67" s="4"/>
+      <c r="AB67" s="4"/>
+      <c r="AC67" s="4"/>
+      <c r="AD67" s="4"/>
+      <c r="AE67" s="4"/>
+    </row>
+    <row r="68" spans="27:31" x14ac:dyDescent="0.3">
+      <c r="AA68" s="4"/>
+      <c r="AB68" s="4"/>
+      <c r="AC68" s="4"/>
+      <c r="AD68" s="4"/>
+      <c r="AE68" s="4"/>
+    </row>
+    <row r="69" spans="27:31" x14ac:dyDescent="0.3">
+      <c r="AA69" s="4"/>
+      <c r="AB69" s="4"/>
+      <c r="AC69" s="4"/>
+      <c r="AD69" s="4"/>
+      <c r="AE69" s="4"/>
+    </row>
+    <row r="70" spans="27:31" x14ac:dyDescent="0.3">
+      <c r="AA70" s="4"/>
+      <c r="AB70" s="4"/>
+      <c r="AC70" s="4"/>
+      <c r="AD70" s="4"/>
+      <c r="AE70" s="4"/>
+    </row>
+    <row r="71" spans="27:31" x14ac:dyDescent="0.3">
+      <c r="AA71" s="4"/>
+      <c r="AB71" s="4"/>
+      <c r="AC71" s="4"/>
+      <c r="AD71" s="4"/>
+      <c r="AE71" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>